<commit_message>
done with detailing kn and dt
</commit_message>
<xml_diff>
--- a/python-api/uploads/Book1.xlsx
+++ b/python-api/uploads/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Defangga Aby Vonega\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF344FD-F69A-4E99-BDA6-DAA744BB7DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B134BEA-EDA1-4654-87D2-1A78850305D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{1FFCA926-FF49-4D28-B303-D85387D0D145}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Unnamed: 0</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
   <si>
     <t>PENERAPAN MODEL PEMBELAJARAN DEMONTRASI UNTUK MENINGKATKAN HASIL BELAJAR TIK SISWA KELAS X SMA NEGERI 1 KAWANGKOAN</t>
   </si>
@@ -54,6 +51,9 @@
   </si>
   <si>
     <t>PENGARUH PEMANFAATAN MEDIA PEMBELAJARAN BERBASIS MULTIMEDIA TERHADAP HASIL BELAJAR TIK SISWA KELAS VIII SMP ADVENT 2 SARIO MANADO</t>
+  </si>
+  <si>
+    <t>Judul Skripsi</t>
   </si>
 </sst>
 </file>
@@ -425,42 +425,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E4C1164-0499-4937-BDC7-E57C4DEF12CB}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="A12" sqref="A12:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>